<commit_message>
coverage report with updated testcases
</commit_message>
<xml_diff>
--- a/app/build/resources/test/DataSetForbabyMdsheet.xlsx
+++ b/app/build/resources/test/DataSetForbabyMdsheet.xlsx
@@ -4,18 +4,83 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="TestCase01"/>
     <sheet r:id="rId2" sheetId="2" name="TestCase02"/>
+    <sheet r:id="rId3" sheetId="3" name="TestCase03"/>
+    <sheet r:id="rId4" sheetId="4" name="Testcase04"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+  <si>
+    <t>GoalName</t>
+  </si>
+  <si>
+    <t>tagetValue</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Reminder</t>
+  </si>
+  <si>
+    <t>Test Goal</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>Every Saturday</t>
+  </si>
+  <si>
+    <t>Every Sunday</t>
+  </si>
+  <si>
+    <t>DoctorName</t>
+  </si>
+  <si>
+    <t>Diagonis</t>
+  </si>
+  <si>
+    <t>MedicineName</t>
+  </si>
+  <si>
+    <t>CourseDuration</t>
+  </si>
+  <si>
+    <t>Regimen</t>
+  </si>
+  <si>
+    <t>Advice</t>
+  </si>
+  <si>
+    <t>Doc Sanjay</t>
+  </si>
+  <si>
+    <t>UnderNutition</t>
+  </si>
+  <si>
+    <t>Cream</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>need more nutritional intake</t>
+  </si>
   <si>
     <t>PatientName</t>
   </si>
@@ -106,13 +171,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -129,7 +200,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -163,6 +234,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -177,57 +255,56 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,27 +610,27 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="15.75">
-      <c r="A1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>27</v>
+      <c r="A1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="15.75">
-      <c r="A2" s="12">
+      <c r="A2" s="15">
         <v>9643243200</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="15">
         <v>596921</v>
       </c>
     </row>
@@ -573,28 +650,216 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="5" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="13" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="10">
+        <v>34</v>
+      </c>
+      <c r="N2" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="O2" s="10">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -606,82 +871,22 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="3">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="6">
-        <v>34</v>
-      </c>
-      <c r="N2" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="O2" s="6">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added appointment and driverSingleton
</commit_message>
<xml_diff>
--- a/app/build/resources/test/DataSetForbabyMdsheet.xlsx
+++ b/app/build/resources/test/DataSetForbabyMdsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="TestCase01"/>
@@ -12,13 +12,56 @@
     <sheet r:id="rId3" sheetId="3" name="TestCase03"/>
     <sheet r:id="rId4" sheetId="4" name="Testcase04"/>
     <sheet r:id="rId5" sheetId="5" name="Testcase05"/>
+    <sheet r:id="rId6" sheetId="6" name="TestCase06"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+  <si>
+    <t>goal</t>
+  </si>
+  <si>
+    <t>NoteCategory</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Clinic</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>fee</t>
+  </si>
+  <si>
+    <t>Test Goal</t>
+  </si>
+  <si>
+    <t>New Categories</t>
+  </si>
+  <si>
+    <t>Test Notes check</t>
+  </si>
+  <si>
+    <t>sample test notes</t>
+  </si>
+  <si>
+    <t>Abhishek Clinic</t>
+  </si>
+  <si>
+    <t>Doc Sanjay</t>
+  </si>
   <si>
     <t>NoteName</t>
   </si>
@@ -53,9 +96,6 @@
     <t>Reminder</t>
   </si>
   <si>
-    <t>Test Goal</t>
-  </si>
-  <si>
     <t>daily</t>
   </si>
   <si>
@@ -83,9 +123,6 @@
     <t>Advice</t>
   </si>
   <si>
-    <t>Doc Sanjay</t>
-  </si>
-  <si>
     <t>UnderNutition</t>
   </si>
   <si>
@@ -119,9 +156,6 @@
     <t>SecondaryMobile</t>
   </si>
   <si>
-    <t>Clinic</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -146,16 +180,16 @@
     <t>Height</t>
   </si>
   <si>
-    <t>Ankit Sharma</t>
+    <t>Anika Sharma</t>
   </si>
   <si>
     <t>2020-10-10</t>
   </si>
   <si>
-    <t>+91 9376543210</t>
-  </si>
-  <si>
-    <t>Male</t>
+    <t>+91 9876543210</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
   <si>
     <t>Father</t>
@@ -164,10 +198,7 @@
     <t>+91 9876543220</t>
   </si>
   <si>
-    <t>Abhishek Clinic</t>
-  </si>
-  <si>
-    <t>Pune</t>
+    <t>Mumbai</t>
   </si>
   <si>
     <t>400001</t>
@@ -205,12 +236,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -221,6 +246,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -278,36 +309,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -319,7 +362,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -630,23 +673,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="15.75">
-      <c r="A1" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>54</v>
+      <c r="A1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="15.75">
-      <c r="A2" s="14">
+      <c r="A2" s="18">
         <v>9643243200</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="18">
         <v>596921</v>
       </c>
     </row>
@@ -662,118 +705,118 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="2" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="2" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="16" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>41</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>48</v>
+        <v>58</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="4">
+        <v>63</v>
+      </c>
+      <c r="M2" s="13">
         <v>34</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="14">
         <v>3.2</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="13">
         <v>50</v>
       </c>
     </row>
@@ -793,59 +836,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5">
         <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -864,45 +907,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5">
         <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -921,9 +964,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -936,16 +1027,46 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4">
+        <v>45582.229166666664</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>